<commit_message>
Adelanto de entendimiento de datos
</commit_message>
<xml_diff>
--- a/202510_Laboratorio 2 - Agrupación_Diccionario_Customer_data.xlsx
+++ b/202510_Laboratorio 2 - Agrupación_Diccionario_Customer_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\dell\Documents\Uniandes\Cursos_2025_10\IN\Laborarorio Agrupación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nataliavillegas/Documents/NOVENO SEMESTRE (2025-1)/BI/BI-Laboratorio2_Agrupacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5612EB27-9563-490E-B264-D1B9D383A950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81EBEE7-EC72-C145-A408-7367784C5D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{912237B1-D28C-43F6-A85F-65AB1CB388A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{912237B1-D28C-43F6-A85F-65AB1CB388A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>Número de meses como cliente</t>
+  </si>
+  <si>
+    <t>NUM</t>
+  </si>
+  <si>
+    <t>Revisar que este en el rango de 0 a 1</t>
+  </si>
+  <si>
+    <t>cateogorica int</t>
   </si>
 </sst>
 </file>
@@ -220,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -230,6 +239,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,20 +577,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F48892-3FFD-4484-A042-98E6149BE8CF}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="137.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="137.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -586,151 +599,217 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D9:D12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>